<commit_message>
final report with graphics
</commit_message>
<xml_diff>
--- a/source/CRUCEVARIABLES.xlsx
+++ b/source/CRUCEVARIABLES.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GUSTAVO 2021\Personal 2021\Coraly2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diebian\CIPCA\faa-encuestas-03-21\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEDB08E-5889-48E2-B5BD-2091226FC3D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="2"/>
+    <workbookView xWindow="-36450" yWindow="5475" windowWidth="28800" windowHeight="4785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -9180,7 +9181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -9740,7 +9741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -43007,13 +43008,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB1"/>
+  <autoFilter ref="A1:AB1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -44083,11 +44084,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>